<commit_message>
Thống kê sách theo năm
Thống kê sách theo năm
</commit_message>
<xml_diff>
--- a/admin/ajax/Thá»‘ng kÃª NXB2 - Nguyá»…n Trá»ng Äáº¡t.xlsx
+++ b/admin/ajax/Thá»‘ng kÃª NXB2 - Nguyá»…n Trá»ng Äáº¡t.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
   <si>
     <t>THỐNG KÊ SÁCH THEO NXB2 - Nguyễn Trọng Đạt</t>
   </si>
@@ -65,6 +65,9 @@
     <t>Nguyễn Trọng Đạt</t>
   </si>
   <si>
+    <t>2017-04-11</t>
+  </si>
+  <si>
     <t>Trí Tuệ Nhân Tạo</t>
   </si>
   <si>
@@ -72,6 +75,9 @@
   </si>
   <si>
     <t>Xuân Quỳnh</t>
+  </si>
+  <si>
+    <t>2017-06-12</t>
   </si>
 </sst>
 </file>
@@ -475,7 +481,7 @@
     <col min="8" max="8" width="4.570313" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="3.427734" bestFit="true" customWidth="true" style="0"/>
     <col min="10" max="10" width="8.140869" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="8.140869" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="12.854004" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -569,7 +575,7 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6" s="5">
         <v>3</v>
@@ -598,25 +604,25 @@
       <c r="J6" s="5">
         <v>40000</v>
       </c>
-      <c r="K6" s="5">
-        <v>40000</v>
+      <c r="K6" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B7" s="5">
         <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>15</v>
@@ -633,8 +639,8 @@
       <c r="J7" s="5">
         <v>123000</v>
       </c>
-      <c r="K7" s="5">
-        <v>123000</v>
+      <c r="K7" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>